<commit_message>
Adicionada painel da aula
</commit_message>
<xml_diff>
--- a/Dados/IBGE/tabela6579.xlsx
+++ b/Dados/IBGE/tabela6579.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proforlandosantos\Curso-de-Power-BI\Dados\IBGE\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="192" yWindow="48" windowWidth="13332" windowHeight="4200" activeTab="0"/>
+    <workbookView xWindow="190" yWindow="50" windowWidth="13330" windowHeight="4200"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabela" sheetId="1" r:id="rId3"/>
-    <sheet name="Notas" sheetId="2" r:id="rId4"/>
+    <sheet name="Tabela" sheetId="1" r:id="rId1"/>
+    <sheet name="Notas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="190">
   <si>
     <t>Tabela 6579 - População residente estimada</t>
   </si>
@@ -325,40 +330,31 @@
   </si>
   <si>
     <t>4 - Por determinação judicial, os municípios de Livramento e Taperoá, do estado da Paraíba, tiveram seus limites territoriais alterados passando a vigorar, para efeitos de distribuição do Fundo de Participação dos Municípios, as populações de 7.248 e 15.316 habitantes, respectivamente. Processo Judicial nº 0000301-96.2006.4.05.8200 - Tribunal de Justiça da Paraíba.
-Em 2017:
-</t>
-  </si>
-  <si>
-    <t>1 - População judicial do município de Porto Velho-RO: 494.013 habitantes. Processo Judicial nº 12316-40.2016.4.01.4100 - Seção Judiciária de Rondônia.
-</t>
-  </si>
-  <si>
-    <t>2 - População judicial do município de Santa Isabel do Rio Negro-AM: entre 23.773 e 30.564 habitantes. Parecer de Força Executória nº 00007/2017/NUCOB-GEAC/PFAM/PGF/AGU, em trâmite na 3ª VF/AM.
-</t>
-  </si>
-  <si>
-    <t>3 - População judicial do município de Urucará-AM: entre 16.981 e 23.772 habitantes. Parecer de Força Executória nº 00004/2017/NUCOB-GEAC/PFAM/PGF/AGU, em trâmite na 3ª VF/AM.
-</t>
-  </si>
-  <si>
-    <t>4 - População judicial do município de Jacareacanga-PA: 41.487 habitantes. Processo Judicial nº 798-41.2011.4.01.3902, Seção Judiciária de Itaituba-PA.
-</t>
-  </si>
-  <si>
-    <t>5 - População judicial do município de Paço do Lumiar - MA: superior a 156.216 habitantes. Processo Judicial nº13916-98.2017.4.01.3700 - Seção Judiciária do Maranhão- MA.
-</t>
-  </si>
-  <si>
-    <t>6 - População judicial do município Livramento-PB: 7.262 habitantes. Processo Judicial nº 0000301-96.2006.4.05.8200 - Tribunal de Justiça da Paraíba - PB.
-</t>
-  </si>
-  <si>
-    <t>7 - População judicial do município de Taperoá-PB: 15.400 habitantes. Processo Judicial nº 0000301-96.2006.4.05.8200 - Tribunal de Justiça da Paraíba - PB.
-</t>
-  </si>
-  <si>
-    <t>8 - População judicial do município Coronel João Sá-BA: 17.422 habitantes. Processo Judicial nº 0002222-53.2017.4.01.3306 - Vara Única de Paulo Afonso-BA.
-</t>
+Em 2017:</t>
+  </si>
+  <si>
+    <t>1 - População judicial do município de Porto Velho-RO: 494.013 habitantes. Processo Judicial nº 12316-40.2016.4.01.4100 - Seção Judiciária de Rondônia.</t>
+  </si>
+  <si>
+    <t>2 - População judicial do município de Santa Isabel do Rio Negro-AM: entre 23.773 e 30.564 habitantes. Parecer de Força Executória nº 00007/2017/NUCOB-GEAC/PFAM/PGF/AGU, em trâmite na 3ª VF/AM.</t>
+  </si>
+  <si>
+    <t>3 - População judicial do município de Urucará-AM: entre 16.981 e 23.772 habitantes. Parecer de Força Executória nº 00004/2017/NUCOB-GEAC/PFAM/PGF/AGU, em trâmite na 3ª VF/AM.</t>
+  </si>
+  <si>
+    <t>4 - População judicial do município de Jacareacanga-PA: 41.487 habitantes. Processo Judicial nº 798-41.2011.4.01.3902, Seção Judiciária de Itaituba-PA.</t>
+  </si>
+  <si>
+    <t>5 - População judicial do município de Paço do Lumiar - MA: superior a 156.216 habitantes. Processo Judicial nº13916-98.2017.4.01.3700 - Seção Judiciária do Maranhão- MA.</t>
+  </si>
+  <si>
+    <t>6 - População judicial do município Livramento-PB: 7.262 habitantes. Processo Judicial nº 0000301-96.2006.4.05.8200 - Tribunal de Justiça da Paraíba - PB.</t>
+  </si>
+  <si>
+    <t>7 - População judicial do município de Taperoá-PB: 15.400 habitantes. Processo Judicial nº 0000301-96.2006.4.05.8200 - Tribunal de Justiça da Paraíba - PB.</t>
+  </si>
+  <si>
+    <t>8 - População judicial do município Coronel João Sá-BA: 17.422 habitantes. Processo Judicial nº 0002222-53.2017.4.01.3306 - Vara Única de Paulo Afonso-BA.</t>
   </si>
   <si>
     <t>9 - População judicial do município Ibiassucê-BA: entre 10.189 e 13.584 habitantes. Processo Judicial  nº 1018608-53.2017.4.01.3400  (14ª VARA FEDERAL CÍVEL DA SJDF).</t>
@@ -575,8 +571,7 @@
     <t>31 - População judicial do Município de Ribeirão do Pinhal-PR: 13.601 habitantes. Processo Judicial nº 5001464-05.2018.4.04.7013 – Tribunal Regional Federal da 4ª Região.
 De 2018 a 2021:
 As diferenças entre as populações das Unidades da Federação obtidas da soma das estimativas municipais e aquelas projetadas nas Projeções de População, Brasil e Unidades da Federação, Revisão 2018, devem-se à alteração de limites territoriais ocorridas entre os estados, após o Censo Demográfico 2010. 
-Para o histórico de alterações, consulte o link https://www.ibge.gov.br/estatisticas-novoportal/sociais/populacao/9103-estimativas-de-populacao.html.
-</t>
+Para o histórico de alterações, consulte o link https://www.ibge.gov.br/estatisticas-novoportal/sociais/populacao/9103-estimativas-de-populacao.html.</t>
   </si>
   <si>
     <t>Legenda</t>
@@ -635,14 +630,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <color indexed="64"/>
     </font>
   </fonts>
   <fills count="2">
@@ -653,7 +648,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -661,26 +656,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -688,44 +669,400 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
       <c r="D4" t="s">
         <v>6</v>
       </c>
@@ -784,7 +1121,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -852,7 +1189,7 @@
         <v>1815278</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -920,7 +1257,7 @@
         <v>906876</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -988,7 +1325,7 @@
         <v>4269995</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1056,7 +1393,7 @@
         <v>652713</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1124,7 +1461,7 @@
         <v>8777124</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1192,7 +1529,7 @@
         <v>877613</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -1260,7 +1597,7 @@
         <v>1607363</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1328,7 +1665,7 @@
         <v>7153262</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1396,7 +1733,7 @@
         <v>3289290</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1464,7 +1801,7 @@
         <v>9240580</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1532,7 +1869,7 @@
         <v>3560903</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -1600,7 +1937,7 @@
         <v>4059905</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1668,7 +2005,7 @@
         <v>9674793</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -1736,7 +2073,7 @@
         <v>3365351</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1804,7 +2141,7 @@
         <v>2338474</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1872,7 +2209,7 @@
         <v>14985284</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -1940,7 +2277,7 @@
         <v>21411923</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -2008,7 +2345,7 @@
         <v>4108508</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -2076,7 +2413,7 @@
         <v>17463349</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -2144,7 +2481,7 @@
         <v>46649132</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -2212,7 +2549,7 @@
         <v>11597484</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2280,7 +2617,7 @@
         <v>7338473</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2348,7 +2685,7 @@
         <v>11466630</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>25</v>
       </c>
@@ -2416,7 +2753,7 @@
         <v>2839188</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>25</v>
       </c>
@@ -2484,7 +2821,7 @@
         <v>3567234</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>25</v>
       </c>
@@ -2552,7 +2889,7 @@
         <v>7206589</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>25</v>
       </c>
@@ -2620,576 +2957,701 @@
         <v>3094325</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="s">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A32:V32"/>
     <mergeCell ref="A1:V1"/>
     <mergeCell ref="A2:V2"/>
     <mergeCell ref="A3:A4"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:V3"/>
-    <mergeCell ref="A32:V32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C116"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B115"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
+      <c r="B4" s="1"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="s">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="s">
+      <c r="B15" s="1"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
+      <c r="B16" s="1"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
+      <c r="B18" s="1"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="s">
+      <c r="B20" s="1"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="s">
+      <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="s">
+      <c r="B22" s="1"/>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="s">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="s">
+      <c r="B24" s="1"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="s">
+      <c r="B25" s="1"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="s">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="s">
+      <c r="B27" s="1"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
+      <c r="B28" s="1"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="s">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="s">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="s">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="s">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="s">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="s">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="s">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="s">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="s">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="s">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="s">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="s">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="s">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
+      <c r="B46" s="1"/>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="1" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
+      <c r="B48" s="1"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
+      <c r="B49" s="1"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
+      <c r="B51" s="1"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
+      <c r="B52" s="1"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
+      <c r="B53" s="1"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
+      <c r="B54" s="1"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55" s="1" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
+      <c r="B55" s="1"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
+      <c r="B56" s="1"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" s="1" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="s">
+      <c r="B57" s="1"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="s">
+      <c r="B58" s="1"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="s">
+      <c r="B59" s="1"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="s">
+      <c r="B60" s="1"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61" s="1" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="s">
+      <c r="B61" s="1"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="s">
+      <c r="B62" s="1"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="s">
+      <c r="B63" s="1"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="s">
+      <c r="B64" s="1"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="s">
+      <c r="B65" s="1"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="s">
+      <c r="B66" s="1"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="1" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="s">
+      <c r="B67" s="1"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="s">
+      <c r="B68" s="1"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="s">
+      <c r="B69" s="1"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="s">
+      <c r="B70" s="1"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71" s="1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="s">
+      <c r="B71" s="1"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="s">
+      <c r="B72" s="1"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73" s="1" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="s">
+      <c r="B73" s="1"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74" s="1" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="s">
+      <c r="B74" s="1"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75" s="1" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="s">
+      <c r="B75" s="1"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76" s="1" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="s">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77" s="1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="s">
+      <c r="B77" s="1"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="s">
+      <c r="B78" s="1"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79" s="1" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="s">
+      <c r="B79" s="1"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="s">
+      <c r="B80" s="1"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="s">
+      <c r="B81" s="1"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="s">
+      <c r="B82" s="1"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="s">
+      <c r="B83" s="1"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="s">
+      <c r="B84" s="1"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="s">
+      <c r="B85" s="1"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="s">
+      <c r="B86" s="1"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" s="1" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="s">
+      <c r="B87" s="1"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="1" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="s">
+      <c r="B88" s="1"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="1" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="s">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="1" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="s">
+      <c r="B90" s="1"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="1" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="s">
+      <c r="B91" s="1"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="s">
+      <c r="B92" s="1"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="1" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="s">
+      <c r="B93" s="1"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="1" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="s">
+      <c r="B94" s="1"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" s="1" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="96">
-      <c r="A96" t="s">
+      <c r="B95" s="1"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="1" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="97">
-      <c r="A97" t="s">
+      <c r="B96" s="1"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="98">
-      <c r="A98" t="s">
+      <c r="B97" s="1"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" s="1" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="99">
-      <c r="A99" t="s">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" s="1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s">
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" s="1" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="101">
-      <c r="A101" t="s">
+      <c r="B100" s="1"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" s="1" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="102">
-      <c r="A102" t="s">
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" s="1" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="103">
-      <c r="A103" t="s">
+      <c r="B102" s="1"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" s="1" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="s">
+      <c r="B103" s="1"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" s="1" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="s">
+      <c r="B104" s="1"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="1" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="s">
+      <c r="B105" s="1"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="s">
-        <v/>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="s">
+      <c r="B106" s="1"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="1"/>
+      <c r="B107" s="1"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" s="1" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="109">
+      <c r="B108" s="1"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>176</v>
       </c>
@@ -3197,7 +3659,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>178</v>
       </c>
@@ -3205,7 +3667,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>180</v>
       </c>
@@ -3213,7 +3675,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>182</v>
       </c>
@@ -3221,7 +3683,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>184</v>
       </c>
@@ -3229,7 +3691,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>186</v>
       </c>
@@ -3237,7 +3699,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>188</v>
       </c>
@@ -3247,6 +3709,105 @@
     </row>
   </sheetData>
   <mergeCells count="108">
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A101:B101"/>
+    <mergeCell ref="A102:B102"/>
+    <mergeCell ref="A103:B103"/>
+    <mergeCell ref="A104:B104"/>
+    <mergeCell ref="A105:B105"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A107:B107"/>
+    <mergeCell ref="A108:B108"/>
+    <mergeCell ref="A91:B91"/>
+    <mergeCell ref="A92:B92"/>
+    <mergeCell ref="A93:B93"/>
+    <mergeCell ref="A94:B94"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A96:B96"/>
+    <mergeCell ref="A97:B97"/>
+    <mergeCell ref="A98:B98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A82:B82"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A84:B84"/>
+    <mergeCell ref="A85:B85"/>
+    <mergeCell ref="A86:B86"/>
+    <mergeCell ref="A87:B87"/>
+    <mergeCell ref="A88:B88"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A90:B90"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A79:B79"/>
+    <mergeCell ref="A80:B80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A72:B72"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="A60:B60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
@@ -3256,105 +3817,6 @@
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="A60:B60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A66:B66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A79:B79"/>
-    <mergeCell ref="A80:B80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="A82:B82"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A84:B84"/>
-    <mergeCell ref="A85:B85"/>
-    <mergeCell ref="A86:B86"/>
-    <mergeCell ref="A87:B87"/>
-    <mergeCell ref="A88:B88"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A90:B90"/>
-    <mergeCell ref="A91:B91"/>
-    <mergeCell ref="A92:B92"/>
-    <mergeCell ref="A93:B93"/>
-    <mergeCell ref="A94:B94"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A96:B96"/>
-    <mergeCell ref="A97:B97"/>
-    <mergeCell ref="A98:B98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A101:B101"/>
-    <mergeCell ref="A102:B102"/>
-    <mergeCell ref="A103:B103"/>
-    <mergeCell ref="A104:B104"/>
-    <mergeCell ref="A105:B105"/>
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A107:B107"/>
-    <mergeCell ref="A108:B108"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>